<commit_message>
001, 002, 003 améliorés pour revue par Hervé
</commit_message>
<xml_diff>
--- a/thématique SI/001 Système/conception/storyboard 001.xlsx
+++ b/thématique SI/001 Système/conception/storyboard 001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Library/Mobile Documents/com~apple~CloudDocs/Documents/pro/ISIS/2023-2024/dev/projet-FENS/thématique SI/001 Système/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Library/Mobile Documents/com~apple~CloudDocs/Documents/pro/ISIS/2023-2024/dev/projet-FENS/thématique SI/001 Système/conception/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFF0298-575E-AF4A-9191-AF928B8AE408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4694AB90-E090-CA4F-9096-0E672A4B9231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="1340" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3589,10 +3589,10 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
- Les répertoires *hors_git/ ne sont plus versionnés L'objectif est de pouvoir y pla er les éléments de montage qui n'ont pas d'intérêt à être versionnés. En particulier car ils sont lourds et peuvent être regénérés facilement.
- Uniformisation des noms des répertoires en snake case.
</commit_message>
<xml_diff>
--- a/thématique SI/001 Système/conception/storyboard 001.xlsx
+++ b/thématique SI/001 Système/conception/storyboard 001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Library/Mobile Documents/com~apple~CloudDocs/Documents/pro/ISIS/2023-2024/dev/projet-FENS/thématique SI/001 Système/conception/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/dev/projet-FENS/thématique SI/001 Système/conception/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4694AB90-E090-CA4F-9096-0E672A4B9231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF40931-2595-4A46-A55B-629B690FCB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="1340" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,9 +227,6 @@
     <t>Savoir représenter  de façon schématique un  système.</t>
   </si>
   <si>
-    <t>Présentation du symbolisme</t>
-  </si>
-  <si>
     <t>Exemple</t>
   </si>
   <si>
@@ -299,10 +296,13 @@
     <t>c080</t>
   </si>
   <si>
-    <t>Pour réaliser sa fonction  un système utilise des éléments en entrées et produit des éléments en sortie.</t>
+    <t>Prenons l'exemple d'un système de production industrielle. La finalité est de produire des biens et services pour répondre aux besoins des consommateurs et des entreprises. Les entrées peuvent être des matières premières, des données informatiques… Les sorties peuvent être les produits manufacturés, des déchets, des données de production…</t>
   </si>
   <si>
-    <t>Prenons l'exemple d'un système de production industrielle. La finalité est de produire des biens et services pour répondre aux besoins des consommateurs et des entreprises. Les entrées peuvent être des matières premières, des données informatiques… Les sorties peuvent être les produits manufacturés, des déchets, des données de production…</t>
+    <t>Pour réaliser sa fonction  un système ouvert utilise des éléments en entrées et produit des éléments en sortie.</t>
+  </si>
+  <si>
+    <t>Système ouvert</t>
   </si>
 </sst>
 </file>
@@ -3589,10 +3589,10 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3643,7 +3643,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -3690,7 +3690,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -3733,7 +3733,7 @@
     <row r="4" spans="1:27" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="3"/>
@@ -3769,7 +3769,7 @@
     <row r="5" spans="1:27" ht="160.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
@@ -3810,7 +3810,7 @@
     <row r="6" spans="1:27" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>0</v>
@@ -3849,10 +3849,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -3884,18 +3884,18 @@
     <row r="8" spans="1:27" ht="145" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
@@ -3920,24 +3920,24 @@
     </row>
     <row r="9" spans="1:27" ht="136.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -3961,24 +3961,24 @@
     </row>
     <row r="10" spans="1:27" ht="183" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>41</v>
-      </c>
       <c r="H10" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -4089,11 +4089,11 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -4124,7 +4124,7 @@
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>

</xml_diff>